<commit_message>
PRG-Tools Wails application. Working for Payroll and Daily Reports.
</commit_message>
<xml_diff>
--- a/backend/test_output/payrollwarnings.xlsx
+++ b/backend/test_output/payrollwarnings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Payroll Warnings</t>
   </si>
@@ -22,64 +22,76 @@
     <t>Equip Log Missing Cost Code</t>
   </si>
   <si>
-    <t>- Gilberto Ortiz 225010 2026-02-13 1009</t>
-  </si>
-  <si>
-    <t>-  225010 2026-02-13 1009</t>
-  </si>
-  <si>
-    <t>-  225010 2026-02-10 1042</t>
-  </si>
-  <si>
-    <t>- Pablo Marin 225034 2026-02-10 1018</t>
-  </si>
-  <si>
-    <t>- Pablo Marin 225034 2026-02-10 1027</t>
-  </si>
-  <si>
-    <t>- Pablo Marin 225034 2026-02-10 2014</t>
-  </si>
-  <si>
-    <t>- Pablo Marin 225034 2026-02-10 3031</t>
-  </si>
-  <si>
-    <t>- Salvador Ortiz 224034 2026-02-13 1013</t>
+    <t>- 225010 Gilberto Ortiz 2026-02-13 1009</t>
+  </si>
+  <si>
+    <t>- 225010  2026-02-13 1009</t>
+  </si>
+  <si>
+    <t>- 225034  2026-02-12 1027</t>
+  </si>
+  <si>
+    <t>- 225034  2026-02-11 1027</t>
+  </si>
+  <si>
+    <t>- 225034  2026-02-10 1027</t>
+  </si>
+  <si>
+    <t>- 225034  2026-02-13 1027</t>
+  </si>
+  <si>
+    <t>- 225034 Pablo Marin 2026-02-10 2014</t>
+  </si>
+  <si>
+    <t>- 225034 Pablo Marin 2026-02-10 3031</t>
+  </si>
+  <si>
+    <t>- 224034 Salvador Ortiz 2026-02-13 1013</t>
   </si>
   <si>
     <t>Equipment log entry with no matching time card entry</t>
   </si>
   <si>
-    <t>- Gilberto Ortiz2250102026-02-11200/500</t>
-  </si>
-  <si>
-    <t>- Gilberto Ortiz2250102026-02-09200/500</t>
-  </si>
-  <si>
-    <t>- Gilberto Ortiz2250102026-02-10200/500</t>
-  </si>
-  <si>
-    <t>- Doug Richards2250102026-02-13200/500</t>
-  </si>
-  <si>
-    <t>- Agustin Avila2250102026-02-09200/200</t>
-  </si>
-  <si>
-    <t>- Agustin Avila2250102026-02-10200/200</t>
-  </si>
-  <si>
-    <t>- Jesus Garcia2250102026-02-13200/500</t>
-  </si>
-  <si>
-    <t>- Salvador Martinez2250102026-02-13200/310</t>
+    <t>- 225010 Gilberto Ortiz 2026-02-11 200/500 1009</t>
+  </si>
+  <si>
+    <t>- 225010 Gilberto Ortiz 2026-02-09 200/500 1009</t>
+  </si>
+  <si>
+    <t>- 225010 Gilberto Ortiz 2026-02-10 200/500 1009</t>
+  </si>
+  <si>
+    <t>- 225010 Doug Richards 2026-02-13 200/500 3026</t>
+  </si>
+  <si>
+    <t>- 225010 Agustin Avila 2026-02-09 200/200 3026</t>
+  </si>
+  <si>
+    <t>- 225010 Agustin Avila 2026-02-10 200/200 3042</t>
+  </si>
+  <si>
+    <t>- 225010 Jesus Garcia 2026-02-13 200/500 1042</t>
+  </si>
+  <si>
+    <t>- 225010 Salvador Martinez 2026-02-13 200/310 1010</t>
   </si>
   <si>
     <t>Equipment log with no operator</t>
   </si>
   <si>
-    <t>- Equip #: 1009 Job: 225010, Date: 2026-02-13</t>
-  </si>
-  <si>
-    <t>- Equip #: 1042 Job: 225010, Date: 2026-02-10</t>
+    <t>- Equip #: 225010 Job: 1009, Date: 2026-02-13</t>
+  </si>
+  <si>
+    <t>- Equip #: 225034 Job: 1027, Date: 2026-02-12</t>
+  </si>
+  <si>
+    <t>- Equip #: 225034 Job: 1027, Date: 2026-02-11</t>
+  </si>
+  <si>
+    <t>- Equip #: 225034 Job: 1027, Date: 2026-02-10</t>
+  </si>
+  <si>
+    <t>- Equip #: 225034 Job: 1027, Date: 2026-02-13</t>
   </si>
 </sst>
 </file>
@@ -457,14 +469,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12"/>
-    <row r="13">
-      <c r="A13" s="2" t="s">
+    <row r="12">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
+    <row r="13"/>
     <row r="14">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -503,14 +515,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22"/>
-    <row r="23">
-      <c r="A23" s="2" t="s">
+    <row r="22">
+      <c r="A22" t="s">
         <v>19</v>
       </c>
     </row>
+    <row r="23"/>
     <row r="24">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -519,6 +531,26 @@
         <v>21</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>